<commit_message>
Push the correction results with BFO decision criterias
</commit_message>
<xml_diff>
--- a/ESPR_BFO_Classifications_Final.xlsx
+++ b/ESPR_BFO_Classifications_Final.xlsx
@@ -5,42 +5,43 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhooe-my.sharepoint.com/personal/p42770_fhooe_at/Documents/Desktop/DPP_Publication/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhooe-my.sharepoint.com/personal/p42770_fhooe_at/Documents/Dokumente/GitHub/ISM2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="8_{1918ADE5-93D0-4E8B-8B12-260BD63ADD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02F339C3-5CE8-49C3-B007-7E3EEDFC378F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DF8DEF7-2FA2-490C-9979-07E7E3ECC57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="926" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Terminological_Analysis_Results" sheetId="30" r:id="rId1"/>
-    <sheet name="Annotations" sheetId="1" r:id="rId2"/>
-    <sheet name="BFO_List" sheetId="3" r:id="rId3"/>
-    <sheet name="CarbonFootPrint" sheetId="2" r:id="rId4"/>
-    <sheet name="Concentration" sheetId="4" r:id="rId5"/>
-    <sheet name="Disassembly" sheetId="5" r:id="rId6"/>
-    <sheet name="Disposal" sheetId="6" r:id="rId7"/>
-    <sheet name="Durability" sheetId="7" r:id="rId8"/>
-    <sheet name="Energy Consumption" sheetId="8" r:id="rId9"/>
-    <sheet name="Environmental FootPrint" sheetId="9" r:id="rId10"/>
-    <sheet name="Hazardous Waste" sheetId="11" r:id="rId11"/>
-    <sheet name="Installation" sheetId="12" r:id="rId12"/>
-    <sheet name="Maintenance" sheetId="13" r:id="rId13"/>
-    <sheet name="Material Foot Print" sheetId="14" r:id="rId14"/>
-    <sheet name="Nano Plastic Relase" sheetId="16" r:id="rId15"/>
-    <sheet name="Packaging Waste" sheetId="17" r:id="rId16"/>
-    <sheet name="Plastic Waste" sheetId="18" r:id="rId17"/>
-    <sheet name="Recyling" sheetId="19" r:id="rId18"/>
-    <sheet name="Refurbishment" sheetId="20" r:id="rId19"/>
-    <sheet name="Reliability" sheetId="21" r:id="rId20"/>
-    <sheet name="Repair" sheetId="22" r:id="rId21"/>
-    <sheet name="Reuse" sheetId="23" r:id="rId22"/>
-    <sheet name="Safe Use" sheetId="24" r:id="rId23"/>
-    <sheet name="Technical Specification" sheetId="25" r:id="rId24"/>
-    <sheet name="Threshold" sheetId="26" r:id="rId25"/>
-    <sheet name="Type" sheetId="27" r:id="rId26"/>
-    <sheet name="Volume" sheetId="28" r:id="rId27"/>
-    <sheet name="Weight" sheetId="29" r:id="rId28"/>
+    <sheet name="BFO_Decision_Criteria" sheetId="31" r:id="rId1"/>
+    <sheet name="Terminological_Analysis_Results" sheetId="30" r:id="rId2"/>
+    <sheet name="Annotations" sheetId="1" r:id="rId3"/>
+    <sheet name="BFO_List" sheetId="3" r:id="rId4"/>
+    <sheet name="CarbonFootPrint" sheetId="2" r:id="rId5"/>
+    <sheet name="Concentration" sheetId="4" r:id="rId6"/>
+    <sheet name="Disassembly" sheetId="5" r:id="rId7"/>
+    <sheet name="Disposal" sheetId="6" r:id="rId8"/>
+    <sheet name="Durability" sheetId="7" r:id="rId9"/>
+    <sheet name="Energy Consumption" sheetId="8" r:id="rId10"/>
+    <sheet name="Environmental FootPrint" sheetId="9" r:id="rId11"/>
+    <sheet name="Hazardous Waste" sheetId="11" r:id="rId12"/>
+    <sheet name="Installation" sheetId="12" r:id="rId13"/>
+    <sheet name="Maintenance" sheetId="13" r:id="rId14"/>
+    <sheet name="Material Foot Print" sheetId="14" r:id="rId15"/>
+    <sheet name="Nano Plastic Relase" sheetId="16" r:id="rId16"/>
+    <sheet name="Packaging Waste" sheetId="17" r:id="rId17"/>
+    <sheet name="Plastic Waste" sheetId="18" r:id="rId18"/>
+    <sheet name="Recyling" sheetId="19" r:id="rId19"/>
+    <sheet name="Refurbishment" sheetId="20" r:id="rId20"/>
+    <sheet name="Reliability" sheetId="21" r:id="rId21"/>
+    <sheet name="Repair" sheetId="22" r:id="rId22"/>
+    <sheet name="Reuse" sheetId="23" r:id="rId23"/>
+    <sheet name="Safe Use" sheetId="24" r:id="rId24"/>
+    <sheet name="Technical Specification" sheetId="25" r:id="rId25"/>
+    <sheet name="Threshold" sheetId="26" r:id="rId26"/>
+    <sheet name="Type" sheetId="27" r:id="rId27"/>
+    <sheet name="Volume" sheetId="28" r:id="rId28"/>
+    <sheet name="Weight" sheetId="29" r:id="rId29"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="396">
   <si>
     <t>annotationProperty</t>
   </si>
@@ -1240,9 +1241,6 @@
 </t>
   </si>
   <si>
-    <t>Only Relevant ESPR Quotes</t>
-  </si>
-  <si>
     <t>bfo:Site</t>
   </si>
   <si>
@@ -1517,6 +1515,73 @@
   </si>
   <si>
     <t xml:space="preserve"> Information-Reality Distinction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is it a material entity? It must be composed of matter.
+Does it possess causal unity? Are its parts bound together such that they behave as a single, coherent whole?
+Is it maximally self-connected? Is it the entire such unified whole, or is it merely a part of a larger one?
+</t>
+  </si>
+  <si>
+    <t>bfo:entity</t>
+  </si>
+  <si>
+    <t>Does not need to be physical: An information entity like a plan, or a mathematical entity like the number 7, are included.
+Does not need to be concrete: Universals themselves—such as redness, humanity, or cell—are entities.
+Does not need to be independent: A dependent entity, like the smile on a face or the mass of a rock, cannot exist on its own, but it is an entity nonetheless.
+Does not need to be directly observable: Electrons, genes, and gravitational fields are all perfectly valid entities.</t>
+  </si>
+  <si>
+    <t>bfo:continuant</t>
+  </si>
+  <si>
+    <t>Does the entity exist wholly at every single instant of its existence, or does it unfold through a series of temporal parts or phases?
+(A continuant is always whole; an occurrent is always partial.)
+Does the entity endure through change, maintaining its identity even as it gains or loses parts?
+(A continuant persists; an occurrent is defined by its specific set of parts and cannot change them without becoming a different occurrent.)</t>
+  </si>
+  <si>
+    <t>Related Decision Criteria</t>
+  </si>
+  <si>
+    <t>Related BFO Universals</t>
+  </si>
+  <si>
+    <t>Does the entity serve as a host or bearer for other entities, such as qualities (its color, mass) or roles (its function)?
+Does the entity itself depend on or inhere in any other specific entity for its existence?</t>
+  </si>
+  <si>
+    <t>Is the existence of this entity irrevocably tied to a specific, particular bearer?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Does the entity c exist in its bearer in a fully realized, exhibited, or manifested state whenever its bearer exists?
+Does the entity c exist by inhering in one or more independent continuants?</t>
+  </si>
+  <si>
+    <t>Is the existence of this realizable entity c a direct consequence of the internal physical constitution of its bearer? Specifically, if this entity c were to be removed from its bearer, would the bearer, as a matter of necessity, have to undergo a physical change?
+Is there a specific type of process (a realization) that this entity c brings about when its bearer is exposed to a specific type of trigger?</t>
+  </si>
+  <si>
+    <t>Is this entity c bound to one specific, particular bearer, or can its very same instance exist by being instantiated in multiple, distinct bearers, either sequentially or simultaneously?
+Does the entity c require a physical concretization in the form of a specifically dependent continuant in order to exist in the world?</t>
+  </si>
+  <si>
+    <t>Is the entity c constituted of some portion of matter?
+ Does the entity c occupy a three-dimensional spatial region?</t>
+  </si>
+  <si>
+    <t>Is the entity c a three-dimensional (volumetric) space that is defined and bounded by the interior surface(s) of a material entity?
+Is the entity c mobile? Can it change its absolute location in space?</t>
+  </si>
+  <si>
+    <t>Does the entity c unfold through time by being constituted of a succession of different temporal parts or phases?
+Does the existence of the entity c depend on at least one material entity that participates in it?</t>
+  </si>
+  <si>
+    <t>Only Relevant ESPR Quote List</t>
+  </si>
+  <si>
+    <t>UNCLASSIFIED TERM</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1638,9 +1703,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1656,6 +1728,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF775049"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1665,6 +1742,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>442912</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1495425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>199495</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1313717</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AD5AAD9-DF4C-F0AB-5E84-A5CE797BD8E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9967912" y="3805238"/>
+          <a:ext cx="9043458" cy="6176229"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1951,11 +2083,933 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F28BB2-33DE-4FF4-B4F0-EDEF4ED57B15}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="65.28515625" customWidth="1"/>
+    <col min="2" max="2" width="77.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE76926-A2FF-4D6C-9505-0B1518A04EFF}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="81.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="96.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8DEA3A47-D61E-43AA-8574-DAA3BB6259FB}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB09737-6CCB-414E-897A-9707D1A002BA}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="161.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3DF620A-C003-4172-8BD5-6E61936E8E13}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B12</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91A84DD-9E7B-41E0-9228-D99C393E958B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71.7109375" customWidth="1"/>
+    <col min="2" max="2" width="62.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{651E6358-9644-47E8-BD33-3738E9FDA2A3}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1 B3:B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C7BDBE6-8D7A-4E2B-BECC-BB0F5D1D0EC3}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71513F9-0BD5-4941-9A4B-B1DC2422E467}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{824CFCED-73E6-4926-8D61-75E0839E02FE}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF7617F-131E-4E37-8332-E358638760F2}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="80.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7512210A-EDF7-47E6-8AAD-204AD1D7AD42}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD965CA6-A6F6-491B-8212-E9CF7B6B86A7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="111.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FF0C766-40DF-4FF5-A76F-B7C8B776A547}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09FE2DD-CC13-44BA-8C9E-556FD11732B5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBB0E47B-6598-4B82-BCE5-93F41F20D8F2}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F27DB9-7919-4BB9-A3FF-37D8B3361634}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1ED66C51-95FF-4159-A69B-D96DD9979BF4}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1 B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0FFDD1CD-E571-47F1-A33A-B94274799E4E}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9997BA4-8E01-4DC5-9190-7C07C23C8870}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.85546875" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F40311F6-B3AA-4869-9CAE-4151B80181EF}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8910B29B-BCF2-4DFA-A7A8-1949111001DA}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B232CC-0FFD-48F1-932B-6517D6572749}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="131.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{955BE3F7-5438-4A55-8E3E-BDA75E73C215}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B15</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F301C2-E69F-438C-A1AA-0681577DB836}">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,22 +3028,22 @@
         <v>144</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>379</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2003,7 +3057,7 @@
         <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -2020,7 +3074,7 @@
         <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -2034,7 +3088,7 @@
         <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2048,7 +3102,7 @@
         <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -2065,7 +3119,7 @@
         <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2087,7 +3141,7 @@
         <v>157</v>
       </c>
       <c r="D8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2101,7 +3155,7 @@
         <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2115,7 +3169,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B10" t="s">
         <v>172</v>
@@ -2124,7 +3178,7 @@
         <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -2147,18 +3201,18 @@
         <v>158</v>
       </c>
       <c r="D11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C12" t="s">
         <v>172</v>
       </c>
       <c r="D12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -2172,7 +3226,7 @@
         <v>172</v>
       </c>
       <c r="D13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -2186,7 +3240,7 @@
         <v>172</v>
       </c>
       <c r="D14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -2200,7 +3254,7 @@
         <v>172</v>
       </c>
       <c r="D15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -2214,7 +3268,7 @@
         <v>154</v>
       </c>
       <c r="D16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -2234,7 +3288,7 @@
         <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
@@ -2245,9 +3299,12 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C18" s="1"/>
+      <c r="D18" s="14" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -2260,7 +3317,7 @@
         <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -2277,7 +3334,7 @@
         <v>172</v>
       </c>
       <c r="D20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -2288,10 +3345,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -2302,13 +3359,13 @@
         <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2319,7 +3376,7 @@
         <v>157</v>
       </c>
       <c r="D23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2327,13 +3384,13 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
+        <v>320</v>
+      </c>
+      <c r="C24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" t="s">
         <v>321</v>
-      </c>
-      <c r="C24" t="s">
-        <v>154</v>
-      </c>
-      <c r="D24" t="s">
-        <v>322</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -2347,23 +3404,26 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C26" t="s">
         <v>157</v>
       </c>
       <c r="D26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B27" t="s">
         <v>172</v>
@@ -2372,7 +3432,7 @@
         <v>154</v>
       </c>
       <c r="D27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
@@ -2395,7 +3455,7 @@
         <v>154</v>
       </c>
       <c r="D28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -2412,7 +3472,7 @@
         <v>154</v>
       </c>
       <c r="D29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2423,7 +3483,7 @@
         <v>172</v>
       </c>
       <c r="D30" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -2440,7 +3500,7 @@
         <v>172</v>
       </c>
       <c r="D31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -2454,7 +3514,7 @@
         <v>154</v>
       </c>
       <c r="D32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2462,13 +3522,13 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C33" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2479,7 +3539,7 @@
         <v>172</v>
       </c>
       <c r="D34" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G34" t="b">
         <v>1</v>
@@ -2490,13 +3550,13 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D35" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,10 +3564,10 @@
         <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -2521,7 +3581,7 @@
         <v>154</v>
       </c>
       <c r="D37" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2543,7 +3603,7 @@
         <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D39" t="s">
         <v>155</v>
@@ -2574,7 +3634,7 @@
         <v>154</v>
       </c>
       <c r="D41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2599,7 +3659,7 @@
         <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2610,7 +3670,7 @@
         <v>172</v>
       </c>
       <c r="D44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -2627,7 +3687,7 @@
         <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
@@ -2647,7 +3707,7 @@
         <v>154</v>
       </c>
       <c r="D46" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2658,7 +3718,7 @@
         <v>154</v>
       </c>
       <c r="D47" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2672,7 +3732,7 @@
         <v>154</v>
       </c>
       <c r="D48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E48" t="b">
         <v>1</v>
@@ -2695,7 +3755,7 @@
         <v>158</v>
       </c>
       <c r="D49" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2709,7 +3769,7 @@
         <v>154</v>
       </c>
       <c r="D50" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -2729,7 +3789,7 @@
         <v>154</v>
       </c>
       <c r="D51" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
@@ -2749,7 +3809,7 @@
         <v>154</v>
       </c>
       <c r="D52" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -2772,7 +3832,7 @@
         <v>154</v>
       </c>
       <c r="D53" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E53" t="b">
         <v>1</v>
@@ -2792,7 +3852,7 @@
         <v>172</v>
       </c>
       <c r="D54" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G54" t="b">
         <v>1</v>
@@ -2809,7 +3869,7 @@
         <v>154</v>
       </c>
       <c r="D55" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2823,7 +3883,7 @@
         <v>154</v>
       </c>
       <c r="D56" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F56" t="b">
         <v>1</v>
@@ -2834,10 +3894,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B57" t="s">
         <v>154</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2851,7 +3914,7 @@
         <v>157</v>
       </c>
       <c r="D58" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2862,18 +3925,18 @@
         <v>154</v>
       </c>
       <c r="D59" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C60" t="s">
         <v>154</v>
       </c>
       <c r="D60" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F60" t="b">
         <v>1</v>
@@ -2884,7 +3947,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B61" t="s">
         <v>157</v>
@@ -2893,18 +3956,18 @@
         <v>157</v>
       </c>
       <c r="D61" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C62" t="s">
         <v>157</v>
       </c>
       <c r="D62" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2918,99 +3981,96 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B68">
         <f>COUNTIF(C1:C63, "*bfo:Generically Dependent Continuant*")</f>
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B69">
         <f>COUNTIF(C1:C63, "*bfo:Quality*")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B70">
         <f>COUNTIF(C1:C63, "*bfo:Disposition*")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B71">
+        <f>COUNTIF(C1:C63, "*bfo:Process*")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="B71">
-        <f>COUNTIF(C1:C64, "*bfo:Process*")</f>
-        <v>11</v>
-      </c>
-      <c r="C71">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>367</v>
       </c>
       <c r="B72">
         <f>COUNTIF(C1:C65, "*bfo:Specifically Dependent Continuant*")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B73">
         <f>COUNTIF(C1:C66, "*bfo:MaterialEntity*")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B74">
         <f>COUNTIF(C1:C67, "*bfo:site*")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B76">
         <f>SUM(B68:B74)</f>
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B78">
         <f>COUNTIF(B1:B62, "*bfo:Generically Dependent Continuant*")</f>
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B79">
         <f>COUNTIF(C12:C73, "*bfo:Quality*")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B80">
         <f>COUNTIF(C13:C74, "*bfo:Disposition*")</f>
@@ -3019,7 +4079,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B81">
         <f>COUNTIF(B1:B62, "*bfo:Process*")</f>
@@ -3028,7 +4088,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B82">
         <f>COUNTIF(B1:B62, "*bfo:Specifically Dependent Continuant*")</f>
@@ -3037,7 +4097,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B83">
         <f>COUNTIF(B1:B62, "*bfo:MaterialEntity*")</f>
@@ -3046,7 +4106,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B84">
         <f>COUNTIF(B1:B62, "*bfo:Site*")</f>
@@ -3075,7 +4135,7 @@
       <formula>$A1=$B1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F20 E21 E22:F62 G2:G62" xr:uid="{8E5AA307-82B2-4DB7-A456-3DB1CF8D7C9F}">
       <formula1>$A$92:$A$93</formula1>
     </dataValidation>
@@ -3147,7 +4207,7 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId62"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{335074FF-6003-454B-BC7C-DE23F1E0D030}">
           <x14:formula1>
             <xm:f>BFO_List!$A$1:$A$8</xm:f>
@@ -3172,742 +4232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB09737-6CCB-414E-897A-9707D1A002BA}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="161.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3DF620A-C003-4172-8BD5-6E61936E8E13}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B12</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91A84DD-9E7B-41E0-9228-D99C393E958B}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="71.7109375" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{651E6358-9644-47E8-BD33-3738E9FDA2A3}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1 B3:B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C7BDBE6-8D7A-4E2B-BECC-BB0F5D1D0EC3}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71513F9-0BD5-4941-9A4B-B1DC2422E467}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="75.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{824CFCED-73E6-4926-8D61-75E0839E02FE}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B5</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF7617F-131E-4E37-8332-E358638760F2}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="80.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7512210A-EDF7-47E6-8AAD-204AD1D7AD42}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B11</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD965CA6-A6F6-491B-8212-E9CF7B6B86A7}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="111.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FF0C766-40DF-4FF5-A76F-B7C8B776A547}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09FE2DD-CC13-44BA-8C9E-556FD11732B5}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBB0E47B-6598-4B82-BCE5-93F41F20D8F2}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F27DB9-7919-4BB9-A3FF-37D8B3361634}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="89.85546875" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1ED66C51-95FF-4159-A69B-D96DD9979BF4}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1 B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0FFDD1CD-E571-47F1-A33A-B94274799E4E}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9997BA4-8E01-4DC5-9190-7C07C23C8870}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="46.85546875" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F40311F6-B3AA-4869-9CAE-4151B80181EF}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8910B29B-BCF2-4DFA-A7A8-1949111001DA}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B232CC-0FFD-48F1-932B-6517D6572749}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="131.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{955BE3F7-5438-4A55-8E3E-BDA75E73C215}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B15</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0795038-BCF9-4CB6-B80B-A7907B31A32E}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -4050,12 +4375,912 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50079BB-247F-484E-91F7-F04DF67AC07B}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="137.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F2E7428-F43A-4834-BF1C-5DA595B45540}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FED290-F780-4045-BE72-100BD3714DE8}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="195.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77E45BFC-66CA-4D8D-A635-8587284E0EDE}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724BEB0F-ACEC-404F-9DD0-F6F8AE6B71E3}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="149.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{90B4450F-2645-4B66-8365-9E5AB83D465D}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B19</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782AE8F8-821C-4E57-B171-3687BB49EB8F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="129.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9BF33A2-3165-4778-BF83-F11B24B3BA51}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA355D02-CF48-421F-A3D9-B3D1499FFBA1}">
+  <dimension ref="A2:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="155.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FBF8EF93-0E25-412F-BCC4-3E39252A20E8}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1263058F-725F-465A-AA56-75F2251543F6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="126.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D853E46-D960-4839-8AE5-79EA9DBA6B47}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB02E20-DB30-48F7-A9D0-FB200D49051F}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="152.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99F17BD7-F2B8-44CA-B163-6B5B7206730D}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DBB456-6FD4-4B9D-9B9A-714C1BBDB6CA}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0FC93F6F-AC37-4CFF-9CA3-2DE7F6C08A24}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C7BBA-29BC-46AF-8B3D-DCC0257A33EA}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="119.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DB27CB37-B7A9-4EC8-ACFB-8B280082B6BE}">
+          <x14:formula1>
+            <xm:f>BFO_List!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4079,16 +5304,16 @@
         <v>143</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4487,7 +5712,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E25" s="1">
         <v>12</v>
@@ -4504,7 +5729,7 @@
         <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E26" s="1">
         <v>12</v>
@@ -4519,7 +5744,7 @@
         <v>43</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -4529,7 +5754,7 @@
       </c>
       <c r="B28" s="1"/>
       <c r="D28" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E28" s="1">
         <v>2</v>
@@ -4672,7 +5897,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D37" t="s">
         <v>172</v>
@@ -4724,7 +5949,7 @@
       </c>
       <c r="B40" s="1"/>
       <c r="D40" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E40" s="1">
         <v>2</v>
@@ -4756,7 +5981,7 @@
       </c>
       <c r="B42" s="1"/>
       <c r="D42" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -4776,7 +6001,7 @@
         <v>68</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E43" s="1">
         <v>1144</v>
@@ -4802,7 +6027,7 @@
         <v>71</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E45" s="1"/>
     </row>
@@ -5381,791 +6606,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50079BB-247F-484E-91F7-F04DF67AC07B}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="137.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F2E7428-F43A-4834-BF1C-5DA595B45540}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B8</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FED290-F780-4045-BE72-100BD3714DE8}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="195.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77E45BFC-66CA-4D8D-A635-8587284E0EDE}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B16</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724BEB0F-ACEC-404F-9DD0-F6F8AE6B71E3}">
-  <dimension ref="A1:B19"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="149.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{90B4450F-2645-4B66-8365-9E5AB83D465D}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B19</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782AE8F8-821C-4E57-B171-3687BB49EB8F}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="129.7109375" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9BF33A2-3165-4778-BF83-F11B24B3BA51}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B6</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA355D02-CF48-421F-A3D9-B3D1499FFBA1}">
-  <dimension ref="A2:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="155.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FBF8EF93-0E25-412F-BCC4-3E39252A20E8}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B16</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1263058F-725F-465A-AA56-75F2251543F6}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="126.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D853E46-D960-4839-8AE5-79EA9DBA6B47}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB02E20-DB30-48F7-A9D0-FB200D49051F}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="152.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99F17BD7-F2B8-44CA-B163-6B5B7206730D}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B11</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DBB456-6FD4-4B9D-9B9A-714C1BBDB6CA}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF31BA5C-5BA4-461B-9A2A-C813284FA9A4}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -6173,171 +6616,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" customWidth="1"/>
-    <col min="2" max="2" width="73" customWidth="1"/>
+    <col min="1" max="1" width="65.28515625" customWidth="1"/>
+    <col min="2" max="2" width="77.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0FC93F6F-AC37-4CFF-9CA3-2DE7F6C08A24}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1C7BBA-29BC-46AF-8B3D-DCC0257A33EA}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="119.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DB27CB37-B7A9-4EC8-ACFB-8B280082B6BE}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B5</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF31BA5C-5BA4-461B-9A2A-C813284FA9A4}">
-  <dimension ref="A1:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="59.5703125" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -6345,7 +6671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC40C808-33F5-427D-A4DC-E4034C8DFCEB}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -6432,7 +6758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3AF41D-E0A1-4F2D-864F-CEB81CE3AF08}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -6500,7 +6826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94848F02-5932-4576-A62E-4C80B12B6ACC}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -6543,7 +6869,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>166</v>
       </c>
@@ -6551,7 +6877,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>167</v>
       </c>
@@ -6559,7 +6885,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>168</v>
       </c>
@@ -6567,7 +6893,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>171</v>
       </c>
@@ -6592,7 +6918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A127273E-5905-42F7-8611-87BB5D1A71D6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -6655,7 +6981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AD0E95-71FE-4B76-8D8B-C327630DCBD4}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -6812,75 +7138,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE76926-A2FF-4D6C-9505-0B1518A04EFF}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="81.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="96.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8DEA3A47-D61E-43AA-8574-DAA3BB6259FB}">
-          <x14:formula1>
-            <xm:f>BFO_List!$A$1:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>